<commit_message>
- edit report - add api
</commit_message>
<xml_diff>
--- a/School.Financial/ReportSrc/overallreport.xlsx
+++ b/School.Financial/ReportSrc/overallreport.xlsx
@@ -112,7 +112,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -265,47 +265,40 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="14"/>
       <color indexed="8"/>
-      <name val="Cordia New"/>
+      <name val="TH SarabunPSK"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="18"/>
       <color indexed="8"/>
-      <name val="Cordia New"/>
+      <name val="TH SarabunPSK"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="8"/>
-      <name val="Cordia New"/>
+      <name val="TH SarabunPSK"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="16"/>
       <color indexed="8"/>
-      <name val="Cordia New"/>
+      <name val="TH SarabunPSK"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color indexed="8"/>
-      <name val="Cordia New"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
+      <name val="TH SarabunPSK"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -782,68 +775,66 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="18" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="43" fontId="19" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1169,7 +1160,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection sqref="A1:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1177,283 +1168,296 @@
     <col min="1" max="7" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="22.35" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:7" ht="22.35" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="17" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-    </row>
-    <row r="2" spans="1:7" ht="22.35" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="17" t="s">
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+    </row>
+    <row r="2" spans="1:7" ht="22.35" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:7" ht="22.35" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="18" t="s">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:7" ht="22.35" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="4" t="s">
+      <c r="B4" s="8"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="22.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="6" t="s">
+      <c r="B5" s="13"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="15" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="22.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="7">
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="18">
         <v>0</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="18">
         <v>0</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="18">
         <v>0</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="18">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="22.35" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="24" t="s">
+      <c r="A7" s="19"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="24"/>
-      <c r="F7" s="1" t="s">
+      <c r="E7" s="20"/>
+      <c r="F7" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="1"/>
+      <c r="G7" s="19"/>
     </row>
     <row r="8" spans="1:7" ht="22.35" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="25" t="s">
+      <c r="A8" s="19"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="25"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
     </row>
     <row r="9" spans="1:7" ht="22.35" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1" t="s">
+      <c r="A9" s="19"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
     </row>
     <row r="10" spans="1:7" ht="22.35" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
     </row>
     <row r="11" spans="1:7" ht="22.35" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
     </row>
     <row r="12" spans="1:7" ht="22.35" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B12" s="25" t="s">
+      <c r="A12" s="5"/>
+      <c r="B12" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25" t="s">
+      <c r="C12" s="21"/>
+      <c r="D12" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25" t="s">
+      <c r="E12" s="21"/>
+      <c r="F12" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G12" s="25"/>
+      <c r="G12" s="21"/>
     </row>
     <row r="13" spans="1:7" ht="22.35" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B13" s="25" t="s">
+      <c r="A13" s="5"/>
+      <c r="B13" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25" t="s">
+      <c r="C13" s="21"/>
+      <c r="D13" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25" t="s">
+      <c r="E13" s="21"/>
+      <c r="F13" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="G13" s="25"/>
+      <c r="G13" s="21"/>
     </row>
     <row r="14" spans="1:7" ht="22.35" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="16" t="s">
+      <c r="A14" s="19"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="16"/>
-      <c r="F14" s="1" t="s">
+      <c r="E14" s="3"/>
+      <c r="F14" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="1"/>
+      <c r="G14" s="19"/>
     </row>
     <row r="15" spans="1:7" ht="22.35" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="25" t="s">
+      <c r="A15" s="19"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="25"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
     </row>
     <row r="16" spans="1:7" ht="22.35" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="26" t="s">
+      <c r="A16" s="19"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="26"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
     </row>
     <row r="17" spans="1:7" ht="22.35" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-    </row>
-    <row r="18" spans="1:7" s="12" customFormat="1" ht="22.35" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="2" t="s">
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+    </row>
+    <row r="18" spans="1:7" s="2" customFormat="1" ht="22.35" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A18" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="1:7" ht="22.35" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+    </row>
+    <row r="19" spans="1:7" ht="22.35" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A19" s="19"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
     </row>
     <row r="20" spans="1:7" ht="22.35" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="16" t="s">
+      <c r="A20" s="19"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E20" s="16"/>
-      <c r="F20" s="8" t="s">
+      <c r="E20" s="3"/>
+      <c r="F20" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="G20" s="1"/>
+      <c r="G20" s="19"/>
     </row>
     <row r="21" spans="1:7" ht="22.35" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="16" t="s">
+      <c r="A21" s="19"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E21" s="16"/>
-      <c r="F21" s="8" t="s">
+      <c r="E21" s="3"/>
+      <c r="F21" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="G21" s="1"/>
+      <c r="G21" s="19"/>
     </row>
     <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="A17:G17"/>
     <mergeCell ref="D20:E20"/>
@@ -1464,17 +1468,6 @@
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="D15:E15"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="A4:C4"/>
   </mergeCells>
   <pageMargins left="7.874015748031496E-2" right="7.874015748031496E-2" top="0.31496062992125984" bottom="0.31496062992125984" header="0.19685039370078741" footer="0"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>